<commit_message>
Added pictures and css
</commit_message>
<xml_diff>
--- a/WebContent/assets/movies.xlsx
+++ b/WebContent/assets/movies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Pulp Fiction</t>
   </si>
@@ -57,6 +57,21 @@
   </si>
   <si>
     <t>John Hillcoat</t>
+  </si>
+  <si>
+    <t>http://www.gstatic.com/tv/thumb/movieposters/1587/p1587_p_v8_ag.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/M/MV5BNzQzOTk3OTAtNDQ0Zi00ZTVkLWI0MTEtMDllZjNkYzNjNTc4L2ltYWdlXkEyXkFqcGdeQXVyNjU0OTQ0OTY@._V1_SY1000_CR0,0,665,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/M/MV5BMTkxMTA5OTAzMl5BMl5BanBnXkFtZTgwNjA5MDc3NjE@._V1_SY1000_CR0,0,673,1000_AL_.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/M/MV5BMTc0NDQzNTA2Ml5BMl5BanBnXkFtZTcwNzI2OTQzMw@@._V1_.jpg</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/M/MV5BMjAxNjUyNjUwN15BMl5BanBnXkFtZTcwMDgwOTIyOA@@._V1_.jpg</t>
   </si>
 </sst>
 </file>
@@ -378,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -390,7 +405,7 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,8 +415,11 @@
       <c r="C1">
         <v>154</v>
       </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -411,8 +429,11 @@
       <c r="C2">
         <v>136</v>
       </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -422,8 +443,11 @@
       <c r="C3">
         <v>107</v>
       </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -433,8 +457,11 @@
       <c r="C4">
         <v>136</v>
       </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -443,6 +470,9 @@
       </c>
       <c r="C5">
         <v>116</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>